<commit_message>
ReadMe plus fixed stuff
</commit_message>
<xml_diff>
--- a/References Thesis.xlsx
+++ b/References Thesis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merca\Desktop\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merca\Desktop\diadema_ajmc2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8862D12-FF70-4BD8-8135-927011CBF4E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A965A98-DC2E-48D2-BEF1-631863DE8E2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{1BDCB7B3-DD1E-40AD-A9EA-318E7CC7E665}"/>
+    <workbookView xWindow="-21720" yWindow="12435" windowWidth="21840" windowHeight="13290" xr2:uid="{1BDCB7B3-DD1E-40AD-A9EA-318E7CC7E665}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="235">
   <si>
     <t>Agnello, M. 2017. Introductory Chapter: Sea Urchin - Knowledge and Perspectives. Sea Urchin - From Environment to Aquaculture and Biomedicine. doi:10.5772/intechopen.70415</t>
   </si>
@@ -2889,6 +2889,9 @@
   </si>
   <si>
     <t>Gudimova, Elena, et al. “In Vivo Exposure to Northern Diatoms Arrests Sea Urchin Embryonic Development.” Toxicon, vol. 109, 2016, pp. 63–69., doi:10.1016/j.toxicon.2015.11.001.</t>
+  </si>
+  <si>
+    <t>https://bsapubs.onlinelibrary.wiley.com/doi/full/10.3732/apps.1400062</t>
   </si>
 </sst>
 </file>
@@ -2956,13 +2959,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3278,10 +3282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA07B2D-22F0-458D-BD77-D397207C8B6D}">
-  <dimension ref="A1:C236"/>
+  <dimension ref="A1:C238"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A222" sqref="A222"/>
+    <sheetView tabSelected="1" topLeftCell="A216" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -4467,6 +4471,11 @@
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="3"/>
+    </row>
+    <row r="238" spans="1:1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A238" s="4" t="s">
+        <v>234</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A289">
@@ -4487,8 +4496,9 @@
     <hyperlink ref="A91" r:id="rId12" display="https://www.ncbi.nlm.nih.gov/pubmed/26559615" xr:uid="{59653D08-3F4D-4160-84C8-CB1ECCBDBB1F}"/>
     <hyperlink ref="A34" r:id="rId13" display="https://www.ncbi.nlm.nih.gov/pubmed/23453931" xr:uid="{6059E862-7723-4361-A4BE-F83C65562313}"/>
     <hyperlink ref="A208" r:id="rId14" display="https://www.ncbi.nlm.nih.gov/pubmed/26082862" xr:uid="{3AD4F4C2-839C-4A95-9466-2BA7B99D6402}"/>
+    <hyperlink ref="A238" r:id="rId15" xr:uid="{16543972-D561-4FBC-9F9F-4447D16EA95D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added final changes to 16S data along with added metadata categories
</commit_message>
<xml_diff>
--- a/References Thesis.xlsx
+++ b/References Thesis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merca\Desktop\diadema_ajmc2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C56AECE-25EE-433C-9AA1-86D891AF9922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3E2D6E-8726-4B28-8F64-75D9D6E78FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{1BDCB7B3-DD1E-40AD-A9EA-318E7CC7E665}"/>
+    <workbookView xWindow="-10032" yWindow="3330" windowWidth="17280" windowHeight="9102" xr2:uid="{1BDCB7B3-DD1E-40AD-A9EA-318E7CC7E665}"/>
   </bookViews>
   <sheets>
     <sheet name="AllRefs" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="237">
   <si>
     <t>Agnello, M. 2017. Introductory Chapter: Sea Urchin - Knowledge and Perspectives. Sea Urchin - From Environment to Aquaculture and Biomedicine. doi:10.5772/intechopen.70415</t>
   </si>
@@ -1505,6 +1505,1382 @@
   </si>
   <si>
     <r>
+      <t>Young, V. B. (2017). The role of the microbiome in human health and disease: An introduction for clinicians. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bmj</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. doi:10.1136/bmj.j831</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Zeisel, S. H., &amp; Warrier, M. (2017). Trimethylamine N-Oxide, the Microbiome, and Heart and Kidney Disease. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Annual Review of Nutrition,37</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(1), 157-181. doi:10.1146/annurev-nutr-071816-064732</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Zhang, W., Lv, Z., Li, C., Sun, Y., Jiang, H., Zhao, M., . . . Chang, Y. (2019). Transcriptome profiling reveals key roles of phagosome and NOD-like receptor pathway in spotting diseased Strongylocentrotus intermedius. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Fish &amp; Shellfish Immunology,84</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 521-531. doi:10.1016/j.fsi.2018.10.042</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Azzouz, D., Omarbekova, A., Heguy, A., Schwudke, D., Gisch, N., Rovin, B. H., … Silverman, G. J. (2019). Lupus nephritis is linked to disease-activity associated expansions and immunity to a gut commensal. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Annals of the Rheumatic Diseases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>78</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(7), 947–956. doi: 10.1136/annrheumdis-2018-214856</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Bianchini, A., Playle, R. C., Wood, C. M., &amp; Walsh, P. J. (2004). Mechanism of acute silver toxicity in marine invertebrates. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Aquatic Toxicology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(72), 67–82. doi: 10.1016/j.aquatox.2004.11.012</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Gao, Y.-D., Zhao, Y., &amp; Huang, J. (2014). Metabolic Modeling of Common Escherichia coli Strains in Human Gut Microbiome. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Biomed Research International</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. doi: 10.1155/2014/694967</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kubinak, J. L., &amp; Round, J. L. (2016). Do antibodies select a healthy microbiota? </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Nature Reviews Immunology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(12), 767–774. doi: 10.1038/nri.2016.114</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lessios, H. A., Kessing, B. D., &amp; Pearse, J. S. (2001). Population structure and speciation in tropical seas: global phylogeography of the sea urchin Diadema. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Evolution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(5), 955–971. doi: 10.1554/0014-3820(2001)055[0955:psasit]2.0.co;2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Li, B., Li, M., Jin, W., Shui, G., &amp; Speakman, J. (2019). Microbiota Depletion Impairs Thermogenesis of Brown Adipose Tissue and Browning of White Adipose Tissue. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Cell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>26</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(10), 2720–2737. doi: https://doi.org/10.1016/j.celrep.2019.02.015</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Moossavi, S., Sepehri, S., Sears, M., Khafipour, E., &amp; Azad, M. (2019). Composition and Variation of the Human Milk Microbiota Are Influenced by Maternal and Early-Life Factors. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Cell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(2), 324–335. doi: https://doi.org/10.1016/j.chom.2019.01.011</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mumby, P. J. (2006). Fishing, Trophic Cascades, and the Process of Grazing on Coral Reefs. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Science</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>311</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(5757), 98–101. doi: 10.1126/science.1121129</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mumby, P. J. (2006). The Impact Of Exploiting Grazers (Scaridae) On The Dynamics Of Caribbean Coral Reefs. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Ecological Applications</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(2), 747–769. doi: 10.1890/1051-0761(2006)016[0747:tioegs]2.0.co;2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Shi, N., Li, N., Duan, X., &amp; Niu, H. (2017). Interaction between the gut microbiome and mucosal immune system. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Military Medical Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(1). doi: 10.1186/s40779-017-0122-9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Valles-Colomer, M., Falony, G., Darzi, Y., Tigchelaar, E. F., Wang, J., Tito, R. Y., … Raes, J. (2019). The neuroactive potential of the human gut microbiota in quality of life and depression. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Nature Microbiology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(4), 623–632. doi: 10.1038/s41564-018-0337-x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Weil, E., Torres, J. L., &amp; Ashton, M. (2005). Population characteristics of the sea urchin Diadema antillarum in La Parguera, Puerto Rico, 17 years after the mass mortality event. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Revista De Biologia Tropical</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 219–231.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Wilson, M. R., Jiang, Y., Villalta, P. W., Stornetta, A., Boudreau, P. D., Carrá, A., … Balskus, E. P. (2019). The human gut bacterial genotoxin colibactin alkylates DNA. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Science</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>363</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(6428). doi: 10.1126/science.aar7785</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ziegenhorn, M., Zhadan, P., &amp; Vaschenko, M. A. (2017). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sea Urchin - From Environment to Aquaculture and Biomedicine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. InTech. doi: 10.5772/65503</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Levitan, Don R., et al. “What Makes a Species Common? No Evidence of Density-Dependent Recruitment or Mortality of the Sea Urchin Diadema Antillarum after the 1983–1984 Mass Mortality.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Oecologia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 175, no. 1, 2014, pp. 117–128., doi:10.1007/s00442-013-2871-9.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Shang, Xiao-Hui, et al. “Traditional Chinese Medicine——Sea Urchin.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Mini-Reviews in Medicinal Chemistry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 14, no. 6, 2014, pp. 537–542., doi:10.2174/1389557514666140529224147.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gambardella, Chiara, et al. “Review: Morphofunctional and Biochemical Markers of Stress in Sea Urchin Life Stages Exposed to Engineered Nanoparticles.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Environmental Toxicology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 31, no. 11, 2015, pp. 1552–1562., doi:10.1002/tox.22159.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lessios, H.a. “The GreatDiadema AntillarumDie-Off: 30 Years Later.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Annual Review of Marine Science</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 8, no. 1, 2016, pp. 267–283., doi:10.1146/annurev-marine-122414-033857.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Farina, Simone, et al. “The Seagrass Effect Turned Upside Down Changes the Prospective of Sea Urchin Survival and Landscape Implications.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Plos One</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 11, no. 10, 2016, doi:10.1371/journal.pone.0164294.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Feehan, Colette J., et al. “Fertilization Limitation OfDiadema Antillarumon Coral Reefs in the Florida Keys.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Ecology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 97, no. 8, 2016, pp. 1897–1904., doi:10.1002/ecy.1461.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Quistad, Steven D, et al. “Viruses and the Origin of Microbiome Selection and Immunity.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>The ISME Journal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 11, no. 4, 2016, pp. 835–840., doi:10.1038/ismej.2016.182.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kriegisch, Nina, et al. “Phase-Shift Dynamics of Sea Urchin Overgrazing on Nutrified Reefs.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Plos One</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 11, no. 12, 2016, doi:10.1371/journal.pone.0168333.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chotirmall, Sanjay H., et al. “Microbiomes in Respiratory Health and Disease: An Asia-Pacific Perspective.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Respirology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 22, no. 2, 2017, pp. 240–250., doi:10.1111/resp.12971.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Young, Vincent B. “The Role of the Microbiome in Human Health and Disease: an Introduction for Clinicians.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bmj</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 2017, doi:10.1136/bmj.j831.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hay, Mark E., and Phillip R. Taylor. “Competition between Herbivourous Fishes and Urchins on Caribbean Reefs.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Oecologia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 65, no. 4, 1985, pp. 591–598., doi:10.1007/bf00379678.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Neuman, Hadar, and Omry Koren. “The Pregnancy Microbiome.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Intestinal Microbiome: Functional Aspects in Health and Disease Nestlé Nutrition Institute Workshop Series</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 2017, pp. 1–9., doi:10.1159/000455207.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tropini, Carolina, et al. “The Gut Microbiome: Connecting Spatial Organization to Function.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Cell Host &amp; Microbe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 21, no. 4, 2017, pp. 433–442., doi:10.1016/j.chom.2017.03.010.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Blum, Hubert E. “The Human Microbiome.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Advances in Medical Sciences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 62, no. 2, 2017, pp. 414–420., doi:10.1016/j.advms.2017.04.005.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zeisel, Steven H., and Manya Warrier. “TrimethylamineN-Oxide, the Microbiome, and Heart and Kidney Disease.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Annual Review of Nutrition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 37, no. 1, 2017, pp. 157–181., doi:10.1146/annurev-nutr-071816-064732.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Defilippo, John, et al. “Comparison of Phagocytosis in Three Caribbean Sea Urchins.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Developmental &amp; Comparative Immunology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 78, 2018, pp. 14–25., doi:10.1016/j.dci.2017.09.007.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ahmadmehrabi, Shadi, and W.h. Wilson Tang. “Gut Microbiome and Its Role in Cardiovascular Diseases.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Current Opinion in Cardiology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 32, no. 6, 2017, pp. 761–766., doi:10.1097/hco.0000000000000445.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Barko, P.c., et al. “The Gastrointestinal Microbiome: A Review.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Journal of Veterinary Internal Medicine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 32, no. 1, 2017, pp. 9–25., doi:10.1111/jvim.14875.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gorkiewicz, Gregor, and Alexander Moschen. “Gut Microbiome: a New Player in Gastrointestinal Disease.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Virchows Archiv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 472, no. 1, 2017, pp. 159–172., doi:10.1007/s00428-017-2277-x.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Neves, Raquel A.f., et al. “Effects of the Toxic Benthic Dinoflagellate Ostreopsis Cf. Ovata on Fertilization and Early Development of the Sea Urchin Lytechinus Variegatus.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Marine Environmental Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 135, 2018, pp. 11–17., doi:10.1016/j.marenvres.2018.01.014.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Barreras, Ruber Rodriguez, et al. “Understanding Trophic Relationships among Caribbean Sea Urchins.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Revista De Biología Tropical</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 64, no. 2, 2016, p. 837., doi:10.15517/rbt.v64i2.19366.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Farina, S., et al. “Hydrodynamic Patterns Favouring Sea Urchin Recruitment in Coastal Areas: A Mediterranean Study Case.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Marine Environmental Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 139, 2018, pp. 182–192., doi:10.1016/j.marenvres.2018.05.013.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bronstein, Omri, et al. “Mind the Gap! The Mitochondrial Control Region and Its Power as a Phylogenetic Marker in Echinoids.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>BMC Evolutionary Biology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 18, no. 1, 2018, doi:10.1186/s12862-018-1198-x.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rodríguez, Adriana, et al. “Effects of Ocean Acidification on Algae Growth and Feeding Rates of Juvenile Sea Urchins.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Marine Environmental Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 140, 2018, pp. 382–389., doi:10.1016/j.marenvres.2018.07.004.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Láruson, Áki Jarl, et al. “Gene Expression across Tissues, Sex, and Life Stages in the Sea Urchin Tripneustes Gratilla [Toxopneustidae, Odontophora, Camarodonta].” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Marine Genomics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 41, 2018, pp. 12–18., doi:10.1016/j.margen.2018.07.002.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gambardella, Chiara, et al. “Ecotoxicological Effects of Polystyrene Microbeads in a Battery of Marine Organisms Belonging to Different Trophic Levels.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Marine Environmental Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 141, 2018, pp. 313–321., doi:10.1016/j.marenvres.2018.09.023.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Janeiro, Manuel, et al. “Implication of Trimethylamine N-Oxide (TMAO) in Disease: Potential Biomarker or New Therapeutic Target.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Nutrients</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 10, no. 10, 2018, p. 1398., doi:10.3390/nu10101398.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Martony, Molly, et al. “Establishing a Diagnostic Technique for Coelomocentesis in the Long-Spined Sea Urchin Diadema Antillarum.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Journal of Aquatic Animal Health</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 30, no. 4, 2018, pp. 325–331., doi:10.1002/aah.10043.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zhang, Weijie, et al. “Transcriptome Profiling Reveals Key Roles of Phagosome and NOD-like Receptor Pathway in Spotting Diseased Strongylocentrotus Intermedius.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Fish &amp; Shellfish Immunology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 84, 2019, pp. 521–531., doi:10.1016/j.fsi.2018.10.042.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Canyelles, Marina, et al. “Trimethylamine N-Oxide: A Link among Diet, Gut Microbiota, Gene Regulation of Liver and Intestine Cholesterol Homeostasis and HDL Function.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>International Journal of Molecular Sciences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 19, no. 10, 2018, p. 3228., doi:10.3390/ijms19103228.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Koch, Nicolás Mongiardino, et al. “A Phylogenomic Resolution of the Sea Urchin Tree of Life.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>BMC Evolutionary Biology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 18, no. 1, 2018, doi:10.1186/s12862-018-1300-4.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Curren, Emily, and Sandric Chee Yew Leong. “Profiles of Bacterial Assemblages from Microplastics of Tropical Coastal Environments.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Science of The Total Environment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 655, 2019, pp. 313–320., doi:10.1016/j.scitotenv.2018.11.250.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wang, Baohong, et al. “The Human Microbiota in Health and Disease.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Engineering</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 3, no. 1, 2017, pp. 71–82., doi:10.1016/j.eng.2017.01.008.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hall, Michael, and Robert G. Beiko. “16S RRNA Gene Analysis with QIIME2.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Methods in Molecular Biology Microbiome Analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 2018, pp. 113–129., doi:10.1007/978-1-4939-8728-3_8.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estaki, Mehrbod, et al. “QIIME 2 Enables Comprehensive End‐to‐End Analysis of Diverse Microbiome Data and Comparative Studies with Publicly Available Data.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Current Protocols in Bioinformatics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 70, no. 1, 2020, doi:10.1002/cpbi.100.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Varrella, Stefano, et al. “Toxic Diatom Aldehydes Affect Defence Gene Networks in Sea Urchins.” </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Plos One</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, vol. 11, no. 2, 2016, doi:10.1371/journal.pone.0149734.</t>
+    </r>
+  </si>
+  <si>
+    <t>Gudimova, Elena, et al. “In Vivo Exposure to Northern Diatoms Arrests Sea Urchin Embryonic Development.” Toxicon, vol. 109, 2016, pp. 63–69., doi:10.1016/j.toxicon.2015.11.001.</t>
+  </si>
+  <si>
+    <t>https://bsapubs.onlinelibrary.wiley.com/doi/full/10.3732/apps.1400062</t>
+  </si>
+  <si>
+    <r>
       <t>Williams, I. R. (2010). Homeostatic interactions between the intestinal microbiome and the mucosal immune system (LL1-2). </t>
     </r>
     <r>
@@ -1522,1384 +2898,14 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>(Suppl_1_Pt_1), I6-I6. doi:10.1093/intimm/dxq068</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Young, V. B. (2017). The role of the microbiome in human health and disease: An introduction for clinicians. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Bmj</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>. doi:10.1136/bmj.j831</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Zeisel, S. H., &amp; Warrier, M. (2017). Trimethylamine N-Oxide, the Microbiome, and Heart and Kidney Disease. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Annual Review of Nutrition,37</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(1), 157-181. doi:10.1146/annurev-nutr-071816-064732</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Zhang, W., Lv, Z., Li, C., Sun, Y., Jiang, H., Zhao, M., . . . Chang, Y. (2019). Transcriptome profiling reveals key roles of phagosome and NOD-like receptor pathway in spotting diseased Strongylocentrotus intermedius. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Fish &amp; Shellfish Immunology,84</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, 521-531. doi:10.1016/j.fsi.2018.10.042</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Azzouz, D., Omarbekova, A., Heguy, A., Schwudke, D., Gisch, N., Rovin, B. H., … Silverman, G. J. (2019). Lupus nephritis is linked to disease-activity associated expansions and immunity to a gut commensal. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Annals of the Rheumatic Diseases</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>78</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(7), 947–956. doi: 10.1136/annrheumdis-2018-214856</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Bianchini, A., Playle, R. C., Wood, C. M., &amp; Walsh, P. J. (2004). Mechanism of acute silver toxicity in marine invertebrates. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Aquatic Toxicology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>25</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(72), 67–82. doi: 10.1016/j.aquatox.2004.11.012</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Gao, Y.-D., Zhao, Y., &amp; Huang, J. (2014). Metabolic Modeling of Common Escherichia coli Strains in Human Gut Microbiome. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Biomed Research International</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>. doi: 10.1155/2014/694967</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Kubinak, J. L., &amp; Round, J. L. (2016). Do antibodies select a healthy microbiota? </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Nature Reviews Immunology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(12), 767–774. doi: 10.1038/nri.2016.114</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Lessios, H. A., Kessing, B. D., &amp; Pearse, J. S. (2001). Population structure and speciation in tropical seas: global phylogeography of the sea urchin Diadema. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Evolution</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>55</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(5), 955–971. doi: 10.1554/0014-3820(2001)055[0955:psasit]2.0.co;2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Li, B., Li, M., Jin, W., Shui, G., &amp; Speakman, J. (2019). Microbiota Depletion Impairs Thermogenesis of Brown Adipose Tissue and Browning of White Adipose Tissue. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Cell</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>26</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(10), 2720–2737. doi: https://doi.org/10.1016/j.celrep.2019.02.015</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Moossavi, S., Sepehri, S., Sears, M., Khafipour, E., &amp; Azad, M. (2019). Composition and Variation of the Human Milk Microbiota Are Influenced by Maternal and Early-Life Factors. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Cell</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>25</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(2), 324–335. doi: https://doi.org/10.1016/j.chom.2019.01.011</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Mumby, P. J. (2006). Fishing, Trophic Cascades, and the Process of Grazing on Coral Reefs. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Science</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>311</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(5757), 98–101. doi: 10.1126/science.1121129</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Mumby, P. J. (2006). The Impact Of Exploiting Grazers (Scaridae) On The Dynamics Of Caribbean Coral Reefs. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Ecological Applications</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(2), 747–769. doi: 10.1890/1051-0761(2006)016[0747:tioegs]2.0.co;2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Shi, N., Li, N., Duan, X., &amp; Niu, H. (2017). Interaction between the gut microbiome and mucosal immune system. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Military Medical Research</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(1). doi: 10.1186/s40779-017-0122-9</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Valles-Colomer, M., Falony, G., Darzi, Y., Tigchelaar, E. F., Wang, J., Tito, R. Y., … Raes, J. (2019). The neuroactive potential of the human gut microbiota in quality of life and depression. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Nature Microbiology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(4), 623–632. doi: 10.1038/s41564-018-0337-x</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Weil, E., Torres, J. L., &amp; Ashton, M. (2005). Population characteristics of the sea urchin Diadema antillarum in La Parguera, Puerto Rico, 17 years after the mass mortality event. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Revista De Biologia Tropical</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>53</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, 219–231.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Wilson, M. R., Jiang, Y., Villalta, P. W., Stornetta, A., Boudreau, P. D., Carrá, A., … Balskus, E. P. (2019). The human gut bacterial genotoxin colibactin alkylates DNA. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Science</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>363</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(6428). doi: 10.1126/science.aar7785</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Ziegenhorn, M., Zhadan, P., &amp; Vaschenko, M. A. (2017). </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Sea Urchin - From Environment to Aquaculture and Biomedicine</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>. InTech. doi: 10.5772/65503</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Levitan, Don R., et al. “What Makes a Species Common? No Evidence of Density-Dependent Recruitment or Mortality of the Sea Urchin Diadema Antillarum after the 1983–1984 Mass Mortality.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Oecologia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 175, no. 1, 2014, pp. 117–128., doi:10.1007/s00442-013-2871-9.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Shang, Xiao-Hui, et al. “Traditional Chinese Medicine——Sea Urchin.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Mini-Reviews in Medicinal Chemistry</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 14, no. 6, 2014, pp. 537–542., doi:10.2174/1389557514666140529224147.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Gambardella, Chiara, et al. “Review: Morphofunctional and Biochemical Markers of Stress in Sea Urchin Life Stages Exposed to Engineered Nanoparticles.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Environmental Toxicology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 31, no. 11, 2015, pp. 1552–1562., doi:10.1002/tox.22159.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lessios, H.a. “The GreatDiadema AntillarumDie-Off: 30 Years Later.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Annual Review of Marine Science</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 8, no. 1, 2016, pp. 267–283., doi:10.1146/annurev-marine-122414-033857.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Farina, Simone, et al. “The Seagrass Effect Turned Upside Down Changes the Prospective of Sea Urchin Survival and Landscape Implications.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Plos One</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 11, no. 10, 2016, doi:10.1371/journal.pone.0164294.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Feehan, Colette J., et al. “Fertilization Limitation OfDiadema Antillarumon Coral Reefs in the Florida Keys.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Ecology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 97, no. 8, 2016, pp. 1897–1904., doi:10.1002/ecy.1461.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Quistad, Steven D, et al. “Viruses and the Origin of Microbiome Selection and Immunity.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>The ISME Journal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 11, no. 4, 2016, pp. 835–840., doi:10.1038/ismej.2016.182.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Kriegisch, Nina, et al. “Phase-Shift Dynamics of Sea Urchin Overgrazing on Nutrified Reefs.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Plos One</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 11, no. 12, 2016, doi:10.1371/journal.pone.0168333.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Chotirmall, Sanjay H., et al. “Microbiomes in Respiratory Health and Disease: An Asia-Pacific Perspective.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Respirology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 22, no. 2, 2017, pp. 240–250., doi:10.1111/resp.12971.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Young, Vincent B. “The Role of the Microbiome in Human Health and Disease: an Introduction for Clinicians.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Bmj</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, 2017, doi:10.1136/bmj.j831.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hay, Mark E., and Phillip R. Taylor. “Competition between Herbivourous Fishes and Urchins on Caribbean Reefs.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Oecologia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 65, no. 4, 1985, pp. 591–598., doi:10.1007/bf00379678.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Neuman, Hadar, and Omry Koren. “The Pregnancy Microbiome.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Intestinal Microbiome: Functional Aspects in Health and Disease Nestlé Nutrition Institute Workshop Series</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, 2017, pp. 1–9., doi:10.1159/000455207.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tropini, Carolina, et al. “The Gut Microbiome: Connecting Spatial Organization to Function.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Cell Host &amp; Microbe</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 21, no. 4, 2017, pp. 433–442., doi:10.1016/j.chom.2017.03.010.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Blum, Hubert E. “The Human Microbiome.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Advances in Medical Sciences</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 62, no. 2, 2017, pp. 414–420., doi:10.1016/j.advms.2017.04.005.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Zeisel, Steven H., and Manya Warrier. “TrimethylamineN-Oxide, the Microbiome, and Heart and Kidney Disease.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Annual Review of Nutrition</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 37, no. 1, 2017, pp. 157–181., doi:10.1146/annurev-nutr-071816-064732.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Defilippo, John, et al. “Comparison of Phagocytosis in Three Caribbean Sea Urchins.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Developmental &amp; Comparative Immunology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 78, 2018, pp. 14–25., doi:10.1016/j.dci.2017.09.007.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ahmadmehrabi, Shadi, and W.h. Wilson Tang. “Gut Microbiome and Its Role in Cardiovascular Diseases.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Current Opinion in Cardiology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 32, no. 6, 2017, pp. 761–766., doi:10.1097/hco.0000000000000445.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Barko, P.c., et al. “The Gastrointestinal Microbiome: A Review.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Journal of Veterinary Internal Medicine</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 32, no. 1, 2017, pp. 9–25., doi:10.1111/jvim.14875.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Gorkiewicz, Gregor, and Alexander Moschen. “Gut Microbiome: a New Player in Gastrointestinal Disease.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Virchows Archiv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 472, no. 1, 2017, pp. 159–172., doi:10.1007/s00428-017-2277-x.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Neves, Raquel A.f., et al. “Effects of the Toxic Benthic Dinoflagellate Ostreopsis Cf. Ovata on Fertilization and Early Development of the Sea Urchin Lytechinus Variegatus.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Marine Environmental Research</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 135, 2018, pp. 11–17., doi:10.1016/j.marenvres.2018.01.014.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Barreras, Ruber Rodriguez, et al. “Understanding Trophic Relationships among Caribbean Sea Urchins.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Revista De Biología Tropical</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 64, no. 2, 2016, p. 837., doi:10.15517/rbt.v64i2.19366.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Farina, S., et al. “Hydrodynamic Patterns Favouring Sea Urchin Recruitment in Coastal Areas: A Mediterranean Study Case.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Marine Environmental Research</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 139, 2018, pp. 182–192., doi:10.1016/j.marenvres.2018.05.013.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Bronstein, Omri, et al. “Mind the Gap! The Mitochondrial Control Region and Its Power as a Phylogenetic Marker in Echinoids.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>BMC Evolutionary Biology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 18, no. 1, 2018, doi:10.1186/s12862-018-1198-x.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rodríguez, Adriana, et al. “Effects of Ocean Acidification on Algae Growth and Feeding Rates of Juvenile Sea Urchins.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Marine Environmental Research</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 140, 2018, pp. 382–389., doi:10.1016/j.marenvres.2018.07.004.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Láruson, Áki Jarl, et al. “Gene Expression across Tissues, Sex, and Life Stages in the Sea Urchin Tripneustes Gratilla [Toxopneustidae, Odontophora, Camarodonta].” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Marine Genomics</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 41, 2018, pp. 12–18., doi:10.1016/j.margen.2018.07.002.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Gambardella, Chiara, et al. “Ecotoxicological Effects of Polystyrene Microbeads in a Battery of Marine Organisms Belonging to Different Trophic Levels.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Marine Environmental Research</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 141, 2018, pp. 313–321., doi:10.1016/j.marenvres.2018.09.023.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Janeiro, Manuel, et al. “Implication of Trimethylamine N-Oxide (TMAO) in Disease: Potential Biomarker or New Therapeutic Target.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Nutrients</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 10, no. 10, 2018, p. 1398., doi:10.3390/nu10101398.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Martony, Molly, et al. “Establishing a Diagnostic Technique for Coelomocentesis in the Long-Spined Sea Urchin Diadema Antillarum.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Journal of Aquatic Animal Health</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 30, no. 4, 2018, pp. 325–331., doi:10.1002/aah.10043.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Zhang, Weijie, et al. “Transcriptome Profiling Reveals Key Roles of Phagosome and NOD-like Receptor Pathway in Spotting Diseased Strongylocentrotus Intermedius.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Fish &amp; Shellfish Immunology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 84, 2019, pp. 521–531., doi:10.1016/j.fsi.2018.10.042.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Canyelles, Marina, et al. “Trimethylamine N-Oxide: A Link among Diet, Gut Microbiota, Gene Regulation of Liver and Intestine Cholesterol Homeostasis and HDL Function.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>International Journal of Molecular Sciences</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 19, no. 10, 2018, p. 3228., doi:10.3390/ijms19103228.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Koch, Nicolás Mongiardino, et al. “A Phylogenomic Resolution of the Sea Urchin Tree of Life.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>BMC Evolutionary Biology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 18, no. 1, 2018, doi:10.1186/s12862-018-1300-4.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Curren, Emily, and Sandric Chee Yew Leong. “Profiles of Bacterial Assemblages from Microplastics of Tropical Coastal Environments.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Science of The Total Environment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 655, 2019, pp. 313–320., doi:10.1016/j.scitotenv.2018.11.250.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Wang, Baohong, et al. “The Human Microbiota in Health and Disease.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Engineering</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 3, no. 1, 2017, pp. 71–82., doi:10.1016/j.eng.2017.01.008.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hall, Michael, and Robert G. Beiko. “16S RRNA Gene Analysis with QIIME2.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Methods in Molecular Biology Microbiome Analysis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, 2018, pp. 113–129., doi:10.1007/978-1-4939-8728-3_8.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Estaki, Mehrbod, et al. “QIIME 2 Enables Comprehensive End‐to‐End Analysis of Diverse Microbiome Data and Comparative Studies with Publicly Available Data.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Current Protocols in Bioinformatics</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 70, no. 1, 2020, doi:10.1002/cpbi.100.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Varrella, Stefano, et al. “Toxic Diatom Aldehydes Affect Defence Gene Networks in Sea Urchins.” </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Plos One</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, vol. 11, no. 2, 2016, doi:10.1371/journal.pone.0149734.</t>
-    </r>
-  </si>
-  <si>
-    <t>Gudimova, Elena, et al. “In Vivo Exposure to Northern Diatoms Arrests Sea Urchin Embryonic Development.” Toxicon, vol. 109, 2016, pp. 63–69., doi:10.1016/j.toxicon.2015.11.001.</t>
-  </si>
-  <si>
-    <t>https://bsapubs.onlinelibrary.wiley.com/doi/full/10.3732/apps.1400062</t>
+      <t>(Suppl_1_Pt_1), I6-I6. doi:10.10https://www.cambridge.org/core/journals/journal-of-the-marine-biological-association-of-the-united-kingdom/article/revisiting-the-population-status-of-the-sea-urchin-diadema-antillarum-in-northern-puerto-rico/E27E7958C257AF819430A078AD66798993/intimm/dxq068</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/journal-of-the-marine-biological-association-of-the-united-kingdom/article/revisiting-the-population-status-of-the-sea-urchin-diadema-antillarum-in-northern-puerto-rico/E27E7958C257AF819430A078AD667989</t>
+  </si>
+  <si>
+    <t>https://bioone.org/journals/caribbean-journal-of-science/volume-45/issue-1/cjos.v45i1.a14/Temporal-Variation-of-Early-Larval-Stages-of-the-Long-Spined/10.18475/cjos.v45i1.a14.short</t>
   </si>
 </sst>
 </file>
@@ -2967,7 +2973,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2975,6 +2981,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3290,10 +3297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA07B2D-22F0-458D-BD77-D397207C8B6D}">
-  <dimension ref="A1:C238"/>
+  <dimension ref="A1:C239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A224" sqref="A224"/>
+    <sheetView tabSelected="1" topLeftCell="A219" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A239" sqref="A239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -3314,12 +3321,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -3359,7 +3366,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -3374,7 +3381,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -3384,7 +3391,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3409,7 +3416,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3449,7 +3456,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3504,7 +3511,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3539,7 +3546,7 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3594,7 +3601,7 @@
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3619,7 +3626,7 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3654,7 +3661,7 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3664,12 +3671,12 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3679,12 +3686,12 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3719,17 +3726,17 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3739,7 +3746,7 @@
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3754,7 +3761,7 @@
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3779,7 +3786,7 @@
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3799,7 +3806,7 @@
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3879,7 +3886,7 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3914,7 +3921,7 @@
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3924,12 +3931,12 @@
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -3939,7 +3946,7 @@
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4014,7 +4021,7 @@
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4044,7 +4051,7 @@
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4064,7 +4071,7 @@
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4074,7 +4081,7 @@
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4129,7 +4136,7 @@
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4164,7 +4171,7 @@
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4184,12 +4191,12 @@
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4209,7 +4216,7 @@
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4219,7 +4226,7 @@
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4264,7 +4271,7 @@
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4289,7 +4296,7 @@
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4329,7 +4336,7 @@
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4344,7 +4351,7 @@
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4379,12 +4386,12 @@
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4394,12 +4401,12 @@
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4409,7 +4416,7 @@
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4419,7 +4426,7 @@
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="2" t="s">
-        <v>179</v>
+        <v>234</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4429,7 +4436,7 @@
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4439,37 +4446,37 @@
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4480,9 +4487,19 @@
     <row r="236" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="3"/>
     </row>
+    <row r="237" spans="1:1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A237" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
     <row r="238" spans="1:1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A239" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -4505,9 +4522,10 @@
     <hyperlink ref="A34" r:id="rId13" display="https://www.ncbi.nlm.nih.gov/pubmed/23453931" xr:uid="{6059E862-7723-4361-A4BE-F83C65562313}"/>
     <hyperlink ref="A208" r:id="rId14" display="https://www.ncbi.nlm.nih.gov/pubmed/26082862" xr:uid="{3AD4F4C2-839C-4A95-9466-2BA7B99D6402}"/>
     <hyperlink ref="A238" r:id="rId15" xr:uid="{16543972-D561-4FBC-9F9F-4447D16EA95D}"/>
+    <hyperlink ref="A237" r:id="rId16" xr:uid="{5E7D3528-7692-4973-8716-6DDA0E849249}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>